<commit_message>
Add more info to $UBRN
</commit_message>
<xml_diff>
--- a/$URBN.xlsx
+++ b/$URBN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE659F9-4FF3-44A9-97BE-859B17F5D65C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28C16F0-24CB-4167-A73D-26ADC2DB4F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="29145" windowHeight="18900" xr2:uid="{B4C2FF2C-7631-4696-82F5-D86669693FEA}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>$URBN</t>
   </si>
@@ -79,9 +79,6 @@
     <t>Stores</t>
   </si>
   <si>
-    <t>Inv</t>
-  </si>
-  <si>
     <t>Update</t>
   </si>
   <si>
@@ -89,6 +86,12 @@
   </si>
   <si>
     <t>Ratios</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Philadelphia, PA</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -275,6 +278,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -290,6 +295,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -672,10 +683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518257A9-999C-47F2-A32D-1E03DE6CDF17}">
-  <dimension ref="B2:E33"/>
+  <dimension ref="B2:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -695,11 +706,11 @@
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" s="13" t="s">
@@ -754,109 +765,121 @@
       <c r="B12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="20"/>
+      <c r="C12" s="20">
+        <f>C8-C11</f>
+        <v>2412.8663999999999</v>
+      </c>
       <c r="D12" s="6"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="25"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="15"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="16"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="25"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="C23" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="31"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="C24" s="30">
+        <v>1970</v>
+      </c>
+      <c r="D24" s="31"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="31"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="7"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="B27" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="31"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="12"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="25"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="7"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B32:D32"/>
+  <mergeCells count="12">
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B22:D22"/>
@@ -864,6 +887,10 @@
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C24:D24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="259" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>

</xml_diff>

<commit_message>
Add MRQ to $URBN
</commit_message>
<xml_diff>
--- a/$URBN.xlsx
+++ b/$URBN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A28C16F0-24CB-4167-A73D-26ADC2DB4F0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F802D-F840-A245-8597-8E8386120277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="29145" windowHeight="18900" xr2:uid="{B4C2FF2C-7631-4696-82F5-D86669693FEA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29360" windowHeight="18900" xr2:uid="{B4C2FF2C-7631-4696-82F5-D86669693FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
   <si>
     <t>$URBN</t>
   </si>
@@ -85,23 +95,280 @@
     <t>IR</t>
   </si>
   <si>
-    <t>Ratios</t>
-  </si>
-  <si>
     <t>Inventory</t>
   </si>
   <si>
     <t>Philadelphia, PA</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>CoFound</t>
+  </si>
+  <si>
+    <t>Richard Hayne</t>
+  </si>
+  <si>
+    <t>CCO</t>
+  </si>
+  <si>
+    <t>Margaret Hayne</t>
+  </si>
+  <si>
+    <t>Melaine Marein-Efron</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>CoPres</t>
+  </si>
+  <si>
+    <t>Francis Conforti</t>
+  </si>
+  <si>
+    <t>Q222</t>
+  </si>
+  <si>
+    <t>Q122</t>
+  </si>
+  <si>
+    <t>Q322</t>
+  </si>
+  <si>
+    <t>Q422</t>
+  </si>
+  <si>
+    <t>Q421</t>
+  </si>
+  <si>
+    <t>Q321</t>
+  </si>
+  <si>
+    <t>Q221</t>
+  </si>
+  <si>
+    <t>Q121</t>
+  </si>
+  <si>
+    <t>Q420</t>
+  </si>
+  <si>
+    <t>Q320</t>
+  </si>
+  <si>
+    <t>Q220</t>
+  </si>
+  <si>
+    <t>Q120</t>
+  </si>
+  <si>
+    <t>Anthropologie</t>
+  </si>
+  <si>
+    <t>Free People Group</t>
+  </si>
+  <si>
+    <t>Nuuly</t>
+  </si>
+  <si>
+    <t>Menus &amp; Venues</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>COGS</t>
+  </si>
+  <si>
+    <t>Gross Profit</t>
+  </si>
+  <si>
+    <t>SG&amp;A</t>
+  </si>
+  <si>
+    <t>Operating Income</t>
+  </si>
+  <si>
+    <t>Other Loss, Net</t>
+  </si>
+  <si>
+    <t>Pretax Income</t>
+  </si>
+  <si>
+    <t>Taxes</t>
+  </si>
+  <si>
+    <t>Net Income</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>Revenue Y/Y</t>
+  </si>
+  <si>
+    <t>Revenue Q/Q</t>
+  </si>
+  <si>
+    <t>Gross Margin</t>
+  </si>
+  <si>
+    <t>Operating Margin</t>
+  </si>
+  <si>
+    <t>Net Margin</t>
+  </si>
+  <si>
+    <t>Taxes %</t>
+  </si>
+  <si>
+    <t>Metrics &amp; Ratios</t>
+  </si>
+  <si>
+    <t>FY18</t>
+  </si>
+  <si>
+    <t>FY19</t>
+  </si>
+  <si>
+    <t>FY20</t>
+  </si>
+  <si>
+    <t>FY21</t>
+  </si>
+  <si>
+    <t>FY22</t>
+  </si>
+  <si>
+    <t>FY23</t>
+  </si>
+  <si>
+    <t>FY24</t>
+  </si>
+  <si>
+    <t>FY25</t>
+  </si>
+  <si>
+    <t>FY26</t>
+  </si>
+  <si>
+    <t>FY27</t>
+  </si>
+  <si>
+    <t>FY28</t>
+  </si>
+  <si>
+    <t>FY29</t>
+  </si>
+  <si>
+    <t>FY30</t>
+  </si>
+  <si>
+    <t>FY31</t>
+  </si>
+  <si>
+    <t>FY32</t>
+  </si>
+  <si>
+    <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>Marketable Securities</t>
+  </si>
+  <si>
+    <t>A/R</t>
+  </si>
+  <si>
+    <t>Prepaid Expenses &amp; OCA</t>
+  </si>
+  <si>
+    <t>TCA</t>
+  </si>
+  <si>
+    <t>PP&amp;E</t>
+  </si>
+  <si>
+    <t>Operating Lease ROU</t>
+  </si>
+  <si>
+    <t>Deferred Income Taxes</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>Current Operating Lease</t>
+  </si>
+  <si>
+    <t>Accrued Expenses &amp; OCL</t>
+  </si>
+  <si>
+    <t>TCL</t>
+  </si>
+  <si>
+    <t>Non-Current Operating Lease</t>
+  </si>
+  <si>
+    <t>Deferred Rent &amp; Other</t>
+  </si>
+  <si>
+    <t>Liabilities</t>
+  </si>
+  <si>
+    <t>S/E</t>
+  </si>
+  <si>
+    <t>S/E+L</t>
+  </si>
+  <si>
+    <t>Book Value</t>
+  </si>
+  <si>
+    <t>Book Value per Share</t>
+  </si>
+  <si>
+    <t>Share Price</t>
+  </si>
+  <si>
+    <t>Inventory Y/Y</t>
+  </si>
+  <si>
+    <t>Inventory Q/Q</t>
+  </si>
+  <si>
+    <t>Inventory/Revenue</t>
+  </si>
+  <si>
+    <t>P/B</t>
+  </si>
+  <si>
+    <t>P/S</t>
+  </si>
+  <si>
+    <t>EV/S</t>
+  </si>
+  <si>
+    <t>P/E</t>
+  </si>
+  <si>
+    <t>EV/E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="171" formatCode="0.0\x"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +393,63 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="4"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -245,17 +569,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -264,8 +587,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -274,12 +595,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,8 +622,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,8 +634,62 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -381,6 +766,111 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D78C4F5-DDEF-9639-1B8B-A423DCFBE513}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9156700" y="0"/>
+          <a:ext cx="0" cy="14427200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8487CB8-D284-564E-92DF-F942C8A53AAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15481300" y="0"/>
+          <a:ext cx="0" cy="14427200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -683,202 +1173,294 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{518257A9-999C-47F2-A32D-1E03DE6CDF17}">
-  <dimension ref="B2:E34"/>
+  <dimension ref="A2:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5" s="23" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
         <v>26.04</v>
       </c>
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="13" t="s">
+      <c r="D6" s="43"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="19">
-        <v>92.66</v>
-      </c>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="13" t="s">
+      <c r="C7" s="13">
+        <f>'Financial Model'!L19</f>
+        <v>93.041309999999996</v>
+      </c>
+      <c r="D7" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="13">
         <f>C6*C7</f>
-        <v>2412.8663999999999</v>
-      </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="13" t="s">
+        <v>2422.7957124</v>
+      </c>
+      <c r="D8" s="43"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="13" t="s">
+      <c r="C9" s="13">
+        <f>'Financial Model'!L58</f>
+        <v>404.21299999999997</v>
+      </c>
+      <c r="D9" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="13" t="s">
+      <c r="C10" s="13">
+        <f>'Financial Model'!L59</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
+      <c r="C11" s="13">
+        <f>C9-C10</f>
+        <v>404.21299999999997</v>
+      </c>
+      <c r="D11" s="43" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="14">
         <f>C8-C11</f>
-        <v>2412.8663999999999</v>
-      </c>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+        <v>2018.5827124</v>
+      </c>
+      <c r="D12" s="44"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B15" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="24"/>
       <c r="D15" s="25"/>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="15" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A16" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="15" t="s">
+      <c r="C16" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="15"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="29"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="32"/>
+      <c r="B18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="29"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="27"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="23" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="25"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="30" t="s">
+      <c r="C23" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="29"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="28">
+        <v>1970</v>
+      </c>
+      <c r="D24" s="29"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B25" s="5"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="51">
+        <f>'Financial Model'!L35</f>
+        <v>697.47400000000005</v>
+      </c>
+      <c r="D26" s="52"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B28" s="5"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B29" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="50">
+        <v>44796</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B30" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="31"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="30">
-        <v>1970</v>
-      </c>
-      <c r="D24" s="31"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B26" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="7"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="12"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="31"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="23" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="25"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="7"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="18"/>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="48">
+        <f>C6/'Financial Model'!L56</f>
+        <v>1.4191700244612206</v>
+      </c>
+      <c r="D34" s="49"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B35" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B38" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B39" s="5"/>
+      <c r="C39" s="17"/>
+      <c r="D39" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C34:D34"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
@@ -891,26 +1473,795 @@
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C30:D30"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C30" r:id="rId1" xr:uid="{31241F29-A195-4541-AF4E-F36F49A8B77F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="259" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="259" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F678CC-45B7-4E80-A882-6C501346AF50}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AF74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="C33:D34"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:32" s="20" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="21"/>
+      <c r="H2" s="35">
+        <v>44408</v>
+      </c>
+      <c r="J2" s="35">
+        <v>44592</v>
+      </c>
+      <c r="L2" s="35">
+        <v>44773</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="21"/>
+      <c r="L3" s="34">
+        <v>45139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="39">
+        <v>450.59300000000002</v>
+      </c>
+      <c r="L4" s="39">
+        <v>479.22800000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="39">
+        <v>441.61599999999999</v>
+      </c>
+      <c r="L5" s="39">
+        <v>396.44900000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" s="39">
+        <v>249.708</v>
+      </c>
+      <c r="L6" s="39">
+        <v>271.40300000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="39">
+        <v>9.9390000000000001</v>
+      </c>
+      <c r="L7" s="39">
+        <v>28.776</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="39">
+        <v>5.8689999999999998</v>
+      </c>
+      <c r="L8" s="39">
+        <v>7.532</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="38">
+        <f>SUM(H4:H8)</f>
+        <v>1157.7250000000001</v>
+      </c>
+      <c r="L9" s="38">
+        <f>SUM(L4:L8)</f>
+        <v>1183.3879999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="B10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="40">
+        <v>722.46</v>
+      </c>
+      <c r="L10" s="40">
+        <v>808.83600000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="38">
+        <f>H9-H10</f>
+        <v>435.2650000000001</v>
+      </c>
+      <c r="L11" s="38">
+        <f>L9-L10</f>
+        <v>374.55199999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="40">
+        <v>269.41199999999998</v>
+      </c>
+      <c r="L12" s="40">
+        <v>288.73399999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="38">
+        <f>H11-H12</f>
+        <v>165.85300000000012</v>
+      </c>
+      <c r="L13" s="38">
+        <f>L11-L12</f>
+        <v>85.817999999999927</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="40">
+        <v>1.7969999999999999</v>
+      </c>
+      <c r="L14" s="40">
+        <v>2.262</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="B15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="40">
+        <f>H13-H14</f>
+        <v>164.05600000000013</v>
+      </c>
+      <c r="L15" s="40">
+        <f>L13-L14</f>
+        <v>83.555999999999926</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="B16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H16" s="40">
+        <v>36.793999999999997</v>
+      </c>
+      <c r="L16" s="40">
+        <v>24.082999999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="38">
+        <f>H15-H16</f>
+        <v>127.26200000000013</v>
+      </c>
+      <c r="L17" s="38">
+        <f>L15-L16</f>
+        <v>59.472999999999928</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B18" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="41">
+        <f>H17/H19</f>
+        <v>1.2944253588813188</v>
+      </c>
+      <c r="L18" s="41">
+        <f>L17/L19</f>
+        <v>0.63921069039118139</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="42">
+        <v>98.315441000000007</v>
+      </c>
+      <c r="L19" s="42">
+        <v>93.041309999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L21" s="45">
+        <f>L9/H9-1</f>
+        <v>2.216674944395236E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B22" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="46">
+        <f>H11/H9</f>
+        <v>0.37596579498585592</v>
+      </c>
+      <c r="L24" s="46">
+        <f>L11/L9</f>
+        <v>0.31650819511436651</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="46">
+        <f>H13/H9</f>
+        <v>0.14325768209203404</v>
+      </c>
+      <c r="L25" s="46">
+        <f>L13/L9</f>
+        <v>7.2518903352070438E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="46">
+        <f>H17/H9</f>
+        <v>0.10992420479820347</v>
+      </c>
+      <c r="L26" s="46">
+        <f>L17/L9</f>
+        <v>5.0256551528323708E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B27" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H27" s="46">
+        <f>H16/H15</f>
+        <v>0.22427707612034897</v>
+      </c>
+      <c r="L27" s="46">
+        <f>L16/L15</f>
+        <v>0.28822586050074223</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B31" s="47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B32" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="38">
+        <v>464.81099999999998</v>
+      </c>
+      <c r="L32" s="38">
+        <v>91.665000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B33" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" s="38">
+        <v>156.982</v>
+      </c>
+      <c r="L33" s="38">
+        <v>160.02000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B34" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H34" s="40">
+        <v>94.402000000000001</v>
+      </c>
+      <c r="L34" s="40">
+        <v>97.373999999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H35" s="38">
+        <v>483.14800000000002</v>
+      </c>
+      <c r="L35" s="38">
+        <v>697.47400000000005</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="40">
+        <v>196.07</v>
+      </c>
+      <c r="L36" s="40">
+        <v>220.90100000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B37" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="40">
+        <f>SUM(H32:H36)</f>
+        <v>1395.413</v>
+      </c>
+      <c r="L37" s="40">
+        <f>SUM(L32:L36)</f>
+        <v>1267.434</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B38" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H38" s="40">
+        <v>1047.751</v>
+      </c>
+      <c r="L38" s="40">
+        <v>1150.2470000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H39" s="40">
+        <v>1068.9190000000001</v>
+      </c>
+      <c r="L39" s="40">
+        <v>927.68499999999995</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B40" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H40" s="38">
+        <v>113.249</v>
+      </c>
+      <c r="L40" s="38">
+        <v>152.52799999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B41" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H41" s="40">
+        <v>117.556</v>
+      </c>
+      <c r="L41" s="40">
+        <v>155.53800000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B42" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H42" s="40">
+        <f>SUM(H38:H41)+H37</f>
+        <v>3742.8879999999999</v>
+      </c>
+      <c r="L42" s="40">
+        <f>SUM(L38:L41)+L37</f>
+        <v>3653.4319999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="H43" s="40"/>
+      <c r="L43" s="40"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H44" s="40">
+        <v>240.245</v>
+      </c>
+      <c r="L44" s="40">
+        <v>347.80500000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H45" s="40">
+        <v>243.33799999999999</v>
+      </c>
+      <c r="L45" s="40">
+        <v>222.43</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B46" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H46" s="40">
+        <v>462.78199999999998</v>
+      </c>
+      <c r="L46" s="40">
+        <v>396.65</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H47" s="40">
+        <f>SUM(H44:H46)</f>
+        <v>946.36500000000001</v>
+      </c>
+      <c r="L47" s="40">
+        <f>SUM(L44:L46)</f>
+        <v>966.88499999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H48" s="40">
+        <v>1030.212</v>
+      </c>
+      <c r="L48" s="40">
+        <v>868.68600000000004</v>
+      </c>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H49" s="40">
+        <v>96.891000000000005</v>
+      </c>
+      <c r="L49" s="40">
+        <v>110.669</v>
+      </c>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H50" s="40">
+        <f>H47+SUM(H48:H49)</f>
+        <v>2073.4679999999998</v>
+      </c>
+      <c r="L50" s="40">
+        <f>L47+SUM(L48:L49)</f>
+        <v>1946.24</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="H51" s="40"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H52" s="40">
+        <v>1669.42</v>
+      </c>
+      <c r="L52" s="40">
+        <v>1707.192</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H53" s="40">
+        <f>H52+H50</f>
+        <v>3742.8879999999999</v>
+      </c>
+      <c r="L53" s="40">
+        <f>L52+L50</f>
+        <v>3653.4319999999998</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="L54" s="40"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B55" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H55" s="40">
+        <f>H42-H50</f>
+        <v>1669.42</v>
+      </c>
+      <c r="L55" s="40">
+        <f>L42-L50</f>
+        <v>1707.1919999999998</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B56" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H56" s="1">
+        <f>H55/H19</f>
+        <v>16.980242198171087</v>
+      </c>
+      <c r="L56" s="1">
+        <f>L55/L19</f>
+        <v>18.348752828179222</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B58" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="H58" s="39">
+        <f>H32+H33+H40</f>
+        <v>735.04200000000003</v>
+      </c>
+      <c r="L58" s="39">
+        <f>L32+L33+L40</f>
+        <v>404.21299999999997</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12" s="37" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B59" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="40">
+        <f>H58-H59</f>
+        <v>735.04200000000003</v>
+      </c>
+      <c r="L60" s="40">
+        <f>L58-L59</f>
+        <v>404.21299999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L62" s="46">
+        <f>L35/H35-1</f>
+        <v>0.44360320233137673</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B63" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.15">
+      <c r="B64" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H66" s="1">
+        <v>37.18</v>
+      </c>
+      <c r="L66" s="1">
+        <v>20.53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B67" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="40">
+        <f>H66*H19</f>
+        <v>3655.3680963800002</v>
+      </c>
+      <c r="L67" s="40">
+        <f>L66*L19</f>
+        <v>1910.1380942999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B68" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H68" s="40">
+        <f>H67-H60</f>
+        <v>2920.3260963800003</v>
+      </c>
+      <c r="L68" s="40">
+        <f>L67-L60</f>
+        <v>1505.9250943</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" s="53" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="54">
+        <f>AVERAGE(C70:L70)</f>
+        <v>1.6542403839438049</v>
+      </c>
+      <c r="B70" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="H70" s="53">
+        <f>H66/H56</f>
+        <v>2.1896036326269006</v>
+      </c>
+      <c r="L70" s="53">
+        <f>L66/L56</f>
+        <v>1.118877135260709</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B71" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B72" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B73" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="B74" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L1" r:id="rId1" xr:uid="{A150210D-96D1-0642-91C1-FA5095E7FDDD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
+  <ignoredErrors>
+    <ignoredError sqref="L9" formulaRange="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Q322 financial data for $URBN
</commit_message>
<xml_diff>
--- a/$URBN.xlsx
+++ b/$URBN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{758F802D-F840-A245-8597-8E8386120277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417E0EA2-5E4D-4157-8F16-46EBDB2A5FFC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29360" windowHeight="18900" xr2:uid="{B4C2FF2C-7631-4696-82F5-D86669693FEA}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="29355" windowHeight="18900" xr2:uid="{B4C2FF2C-7631-4696-82F5-D86669693FEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -21,22 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
   <si>
     <t>$URBN</t>
   </si>
@@ -357,6 +347,9 @@
   </si>
   <si>
     <t>EV/E</t>
+  </si>
+  <si>
+    <t>Store Impairment</t>
   </si>
 </sst>
 </file>
@@ -365,8 +358,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.0\x"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0\x"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -613,33 +606,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -660,7 +626,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -670,22 +636,49 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="171" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -775,15 +768,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -799,8 +792,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9156700" y="0"/>
-          <a:ext cx="0" cy="14427200"/>
+          <a:off x="8642350" y="0"/>
+          <a:ext cx="0" cy="14312900"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -833,7 +826,7 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>88</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1176,291 +1169,286 @@
   <dimension ref="A2:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="C34" sqref="C34:D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B5" s="23" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>26.04</v>
-      </c>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+        <v>25.53</v>
+      </c>
+      <c r="D6" s="34"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="13">
-        <f>'Financial Model'!L19</f>
-        <v>93.041309999999996</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+        <f>'Financial Model'!M20</f>
+        <v>92.174160000000001</v>
+      </c>
+      <c r="D7" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="13">
         <f>C6*C7</f>
-        <v>2422.7957124</v>
-      </c>
-      <c r="D8" s="43"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+        <v>2353.2063048</v>
+      </c>
+      <c r="D8" s="34"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13">
-        <f>'Financial Model'!L58</f>
-        <v>404.21299999999997</v>
-      </c>
-      <c r="D9" s="43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+        <f>'Financial Model'!M59</f>
+        <v>389.041</v>
+      </c>
+      <c r="D9" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="13">
-        <f>'Financial Model'!L59</f>
+        <f>'Financial Model'!M60</f>
         <v>0</v>
       </c>
-      <c r="D10" s="43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D10" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="13">
         <f>C9-C10</f>
-        <v>404.21299999999997</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+        <v>389.041</v>
+      </c>
+      <c r="D11" s="34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="14">
         <f>C8-C11</f>
-        <v>2018.5827124</v>
-      </c>
-      <c r="D12" s="44"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="B15" s="23" t="s">
+        <v>1964.1653048000001</v>
+      </c>
+      <c r="D12" s="35"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A16" s="32" t="s">
+      <c r="C15" s="47"/>
+      <c r="D15" s="48"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="29"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A17" s="32" t="s">
+      <c r="D16" s="43"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="29"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="32"/>
+      <c r="D17" s="43"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="23"/>
       <c r="B18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="29"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="32" t="s">
+      <c r="D18" s="43"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
         <v>28</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="27"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B22" s="23" t="s">
+      <c r="D19" s="50"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="24"/>
-      <c r="D22" s="25"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="29"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D23" s="43"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="42">
         <v>1970</v>
       </c>
-      <c r="D24" s="29"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D24" s="43"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="5"/>
       <c r="C25" s="15"/>
       <c r="D25" s="16"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="51">
-        <f>'Financial Model'!L35</f>
-        <v>697.47400000000005</v>
+        <f>'Financial Model'!M36</f>
+        <v>743.57899999999995</v>
       </c>
       <c r="D26" s="52"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="28"/>
-      <c r="D27" s="29"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="C27" s="42"/>
+      <c r="D27" s="43"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="7"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="50">
-        <v>44796</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+      <c r="D29" s="39">
+        <v>44887</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="31"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B33" s="23" t="s">
+      <c r="D30" s="54"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="24"/>
-      <c r="D33" s="25"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C33" s="47"/>
+      <c r="D33" s="48"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="48">
-        <f>C6/'Financial Model'!L56</f>
-        <v>1.4191700244612206</v>
-      </c>
-      <c r="D34" s="49"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C34" s="44">
+        <f>C6/'Financial Model'!M57</f>
+        <v>1.3536691715500138</v>
+      </c>
+      <c r="D34" s="45"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="29"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C35" s="42"/>
+      <c r="D35" s="43"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="28"/>
-      <c r="D36" s="29"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C36" s="42"/>
+      <c r="D36" s="43"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="29"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C37" s="42"/>
+      <c r="D37" s="43"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="28"/>
-      <c r="D38" s="29"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="C38" s="42"/>
+      <c r="D38" s="43"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="5"/>
       <c r="C39" s="17"/>
       <c r="D39" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C34:D34"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B15:D15"/>
@@ -1474,6 +1462,11 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C34:D34"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C30" r:id="rId1" xr:uid="{31241F29-A195-4541-AF4E-F36F49A8B77F}"/>
@@ -1486,23 +1479,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F678CC-45B7-4E80-A882-6C501346AF50}">
-  <dimension ref="A1:AF74"/>
+  <dimension ref="A1:AF75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="F43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="S15" sqref="S15"/>
+      <selection pane="bottomRight" activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:32" s="20" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:32" s="20" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C1" s="20" t="s">
         <v>41</v>
       </c>
@@ -1530,10 +1523,10 @@
       <c r="K1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="24" t="s">
         <v>32</v>
       </c>
       <c r="N1" s="20" t="s">
@@ -1585,670 +1578,1053 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="21"/>
-      <c r="H2" s="35">
+      <c r="H2" s="26">
         <v>44408</v>
       </c>
-      <c r="J2" s="35">
+      <c r="I2" s="26">
+        <v>44500</v>
+      </c>
+      <c r="J2" s="26">
         <v>44592</v>
       </c>
-      <c r="L2" s="35">
+      <c r="L2" s="26">
         <v>44773</v>
       </c>
-    </row>
-    <row r="3" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M2" s="26">
+        <v>44500</v>
+      </c>
+    </row>
+    <row r="3" spans="2:32" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21"/>
-      <c r="L3" s="34">
+      <c r="L3" s="25">
         <v>45139</v>
       </c>
-    </row>
-    <row r="4" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="36" t="s">
+      <c r="M3" s="25">
+        <v>44866</v>
+      </c>
+    </row>
+    <row r="4" spans="2:32" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="39">
+      <c r="H4" s="30">
         <v>450.59300000000002</v>
       </c>
-      <c r="L4" s="39">
+      <c r="I4" s="30">
+        <v>431.40699999999998</v>
+      </c>
+      <c r="L4" s="30">
         <v>479.22800000000001</v>
       </c>
-    </row>
-    <row r="5" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="36" t="s">
+      <c r="M4" s="30">
+        <v>484.15800000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="2:32" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="39">
+      <c r="H5" s="30">
         <v>441.61599999999999</v>
       </c>
-      <c r="L5" s="39">
+      <c r="I5" s="30">
+        <v>415.87700000000001</v>
+      </c>
+      <c r="L5" s="30">
         <v>396.44900000000001</v>
       </c>
-    </row>
-    <row r="6" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="36" t="s">
+      <c r="M5" s="30">
+        <v>367.55700000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="39">
+      <c r="H6" s="30">
         <v>249.708</v>
       </c>
-      <c r="L6" s="39">
+      <c r="I6" s="30">
+        <v>264.995</v>
+      </c>
+      <c r="L6" s="30">
         <v>271.40300000000002</v>
       </c>
-    </row>
-    <row r="7" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="36" t="s">
+      <c r="M6" s="30">
+        <v>280.69799999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="39">
+      <c r="H7" s="30">
         <v>9.9390000000000001</v>
       </c>
-      <c r="L7" s="39">
+      <c r="I7" s="30">
+        <v>12.667999999999999</v>
+      </c>
+      <c r="L7" s="30">
         <v>28.776</v>
       </c>
-    </row>
-    <row r="8" spans="2:32" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="36" t="s">
+      <c r="M7" s="30">
+        <v>35.279000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="2:32" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="39">
+      <c r="H8" s="30">
         <v>5.8689999999999998</v>
       </c>
-      <c r="L8" s="39">
+      <c r="I8" s="30">
+        <v>6.4569999999999999</v>
+      </c>
+      <c r="L8" s="30">
         <v>7.532</v>
       </c>
-    </row>
-    <row r="9" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="M8" s="30">
+        <v>7.657</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="29">
         <f>SUM(H4:H8)</f>
         <v>1157.7250000000001</v>
       </c>
-      <c r="L9" s="38">
+      <c r="I9" s="29">
+        <f>SUM(I4:I8)</f>
+        <v>1131.404</v>
+      </c>
+      <c r="L9" s="29">
         <f>SUM(L4:L8)</f>
         <v>1183.3879999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:32" x14ac:dyDescent="0.15">
+      <c r="M9" s="29">
+        <f>SUM(M4:M8)</f>
+        <v>1175.3489999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="40">
+      <c r="H10" s="31">
         <v>722.46</v>
       </c>
-      <c r="L10" s="40">
+      <c r="I10" s="31">
+        <v>740.68600000000004</v>
+      </c>
+      <c r="L10" s="31">
         <v>808.83600000000001</v>
       </c>
-    </row>
-    <row r="11" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="3" t="s">
+      <c r="M10" s="1">
+        <v>817.34799999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H11" s="31">
+        <v>0</v>
+      </c>
+      <c r="I11" s="31">
+        <v>0</v>
+      </c>
+      <c r="L11" s="31">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.95799999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="38">
-        <f>H9-H10</f>
+      <c r="H12" s="29">
+        <f>H9-H10-H11</f>
         <v>435.2650000000001</v>
       </c>
-      <c r="L11" s="38">
-        <f>L9-L10</f>
+      <c r="I12" s="29">
+        <f>I9-I10-I11</f>
+        <v>390.71799999999996</v>
+      </c>
+      <c r="L12" s="29">
+        <f>L9-L10-L11</f>
         <v>374.55199999999991</v>
       </c>
-    </row>
-    <row r="12" spans="2:32" x14ac:dyDescent="0.15">
-      <c r="B12" s="1" t="s">
+      <c r="M12" s="29">
+        <f>M9-M10-M11</f>
+        <v>357.04299999999995</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="40">
+      <c r="H13" s="31">
         <v>269.41199999999998</v>
       </c>
-      <c r="L12" s="40">
+      <c r="I13" s="31">
+        <v>274.83600000000001</v>
+      </c>
+      <c r="L13" s="31">
         <v>288.73399999999998</v>
       </c>
-    </row>
-    <row r="13" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B13" s="3" t="s">
+      <c r="M13" s="1">
+        <v>299.72500000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="2:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="38">
-        <f>H11-H12</f>
+      <c r="H14" s="29">
+        <f>H12-H13</f>
         <v>165.85300000000012</v>
       </c>
-      <c r="L13" s="38">
-        <f>L11-L12</f>
+      <c r="I14" s="29">
+        <f>I12-I13</f>
+        <v>115.88199999999995</v>
+      </c>
+      <c r="L14" s="29">
+        <f>L12-L13</f>
         <v>85.817999999999927</v>
       </c>
-    </row>
-    <row r="14" spans="2:32" x14ac:dyDescent="0.15">
-      <c r="B14" s="1" t="s">
+      <c r="M14" s="29">
+        <f>M12-M13</f>
+        <v>57.317999999999927</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="40">
+      <c r="H15" s="31">
         <v>1.7969999999999999</v>
       </c>
-      <c r="L14" s="40">
+      <c r="I15" s="31">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="L15" s="31">
         <v>2.262</v>
       </c>
-    </row>
-    <row r="15" spans="2:32" x14ac:dyDescent="0.15">
-      <c r="B15" s="1" t="s">
+      <c r="M15" s="1">
+        <v>5.0190000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="40">
-        <f>H13-H14</f>
+      <c r="H16" s="31">
+        <f>H14-H15</f>
         <v>164.05600000000013</v>
       </c>
-      <c r="L15" s="40">
-        <f>L13-L14</f>
+      <c r="I16" s="31">
+        <f>I14-I15</f>
+        <v>115.33099999999995</v>
+      </c>
+      <c r="L16" s="31">
+        <f>L14-L15</f>
         <v>83.555999999999926</v>
       </c>
-    </row>
-    <row r="16" spans="2:32" x14ac:dyDescent="0.15">
-      <c r="B16" s="1" t="s">
+      <c r="M16" s="31">
+        <f>M14-M15</f>
+        <v>52.298999999999928</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="40">
+      <c r="H17" s="31">
         <v>36.793999999999997</v>
       </c>
-      <c r="L16" s="40">
+      <c r="I17" s="31">
+        <v>26.495999999999999</v>
+      </c>
+      <c r="L17" s="31">
         <v>24.082999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B17" s="3" t="s">
+      <c r="M17" s="1">
+        <v>15.068</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H17" s="38">
-        <f>H15-H16</f>
+      <c r="H18" s="29">
+        <f>H16-H17</f>
         <v>127.26200000000013</v>
       </c>
-      <c r="L17" s="38">
-        <f>L15-L16</f>
+      <c r="I18" s="29">
+        <f>I16-I17</f>
+        <v>88.834999999999951</v>
+      </c>
+      <c r="L18" s="29">
+        <f>L16-L17</f>
         <v>59.472999999999928</v>
       </c>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B18" s="1" t="s">
+      <c r="M18" s="29">
+        <f>M16-M17</f>
+        <v>37.230999999999931</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H18" s="41">
-        <f>H17/H19</f>
+      <c r="H19" s="32">
+        <f>H18/H20</f>
         <v>1.2944253588813188</v>
       </c>
-      <c r="L18" s="41">
-        <f>L17/L19</f>
+      <c r="I19" s="32">
+        <f>I18/I20</f>
+        <v>0.90461130180740235</v>
+      </c>
+      <c r="L19" s="32">
+        <f>L18/L20</f>
         <v>0.63921069039118139</v>
       </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B19" s="1" t="s">
+      <c r="M19" s="32">
+        <f>M18/M20</f>
+        <v>0.4039201442139525</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H19" s="42">
+      <c r="H20" s="33">
         <v>98.315441000000007</v>
       </c>
-      <c r="L19" s="42">
+      <c r="I20" s="31">
+        <v>98.202399</v>
+      </c>
+      <c r="L20" s="33">
         <v>93.041309999999996</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B21" s="3" t="s">
+      <c r="M20" s="31">
+        <v>92.174160000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L21" s="45">
+      <c r="L22" s="36">
         <f>L9/H9-1</f>
         <v>2.216674944395236E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B22" s="1" t="s">
+      <c r="M22" s="36">
+        <f t="shared" ref="M22" si="0">M9/I9-1</f>
+        <v>3.8841121297078507E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B24" s="1" t="s">
+      <c r="I23" s="37">
+        <f>I9/H9-1</f>
+        <v>-2.2735105487054486E-2</v>
+      </c>
+      <c r="M23" s="37">
+        <f>M9/L9-1</f>
+        <v>-6.7932072997191062E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H24" s="46">
-        <f>H11/H9</f>
+      <c r="H25" s="37">
+        <f>H12/H9</f>
         <v>0.37596579498585592</v>
       </c>
-      <c r="L24" s="46">
-        <f>L11/L9</f>
+      <c r="I25" s="37">
+        <f t="shared" ref="I25" si="1">I12/I9</f>
+        <v>0.3453390654443505</v>
+      </c>
+      <c r="L25" s="37">
+        <f>L12/L9</f>
         <v>0.31650819511436651</v>
       </c>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B25" s="1" t="s">
+      <c r="M25" s="37">
+        <f t="shared" ref="M25" si="2">M12/M9</f>
+        <v>0.30377615499736671</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="46">
-        <f>H13/H9</f>
+      <c r="H26" s="37">
+        <f>H14/H9</f>
         <v>0.14325768209203404</v>
       </c>
-      <c r="L25" s="46">
-        <f>L13/L9</f>
+      <c r="I26" s="37">
+        <f t="shared" ref="I26" si="3">I14/I9</f>
+        <v>0.10242318393783295</v>
+      </c>
+      <c r="L26" s="37">
+        <f>L14/L9</f>
         <v>7.2518903352070438E-2</v>
       </c>
-    </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B26" s="1" t="s">
+      <c r="M26" s="37">
+        <f t="shared" ref="M26" si="4">M14/M9</f>
+        <v>4.8766791820982473E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="H26" s="46">
-        <f>H17/H9</f>
+      <c r="H27" s="37">
+        <f>H18/H9</f>
         <v>0.10992420479820347</v>
       </c>
-      <c r="L26" s="46">
-        <f>L17/L9</f>
+      <c r="I27" s="37">
+        <f t="shared" ref="I27" si="5">I18/I9</f>
+        <v>7.8517488006052613E-2</v>
+      </c>
+      <c r="L27" s="37">
+        <f>L18/L9</f>
         <v>5.0256551528323708E-2</v>
       </c>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B27" s="1" t="s">
+      <c r="M27" s="37">
+        <f t="shared" ref="M27" si="6">M18/M9</f>
+        <v>3.1676548837834495E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H27" s="46">
-        <f>H16/H15</f>
+      <c r="H28" s="37">
+        <f>H17/H16</f>
         <v>0.22427707612034897</v>
       </c>
-      <c r="L27" s="46">
-        <f>L16/L15</f>
+      <c r="I28" s="37">
+        <f t="shared" ref="I28" si="7">I17/I16</f>
+        <v>0.22973875194006824</v>
+      </c>
+      <c r="L28" s="37">
+        <f>L17/L16</f>
         <v>0.28822586050074223</v>
       </c>
-    </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B31" s="47" t="s">
+      <c r="M28" s="37">
+        <f t="shared" ref="M28" si="8">M17/M16</f>
+        <v>0.28811258341459722</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="38" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="3" t="s">
+    <row r="33" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H32" s="38">
+      <c r="H33" s="29">
         <v>464.81099999999998</v>
       </c>
-      <c r="L32" s="38">
+      <c r="I33" s="29">
+        <v>236.35400000000001</v>
+      </c>
+      <c r="L33" s="29">
         <v>91.665000000000006</v>
       </c>
-    </row>
-    <row r="33" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B33" s="3" t="s">
+      <c r="M33" s="29">
+        <v>147.43100000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H33" s="38">
+      <c r="H34" s="29">
         <v>156.982</v>
       </c>
-      <c r="L33" s="38">
+      <c r="I34" s="29">
+        <v>188.375</v>
+      </c>
+      <c r="L34" s="29">
         <v>160.02000000000001</v>
       </c>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B34" s="1" t="s">
+      <c r="M34" s="29">
+        <v>146.364</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H35" s="31">
         <v>94.402000000000001</v>
       </c>
-      <c r="L34" s="40">
+      <c r="I35" s="31">
+        <v>114.208</v>
+      </c>
+      <c r="L35" s="31">
         <v>97.373999999999995</v>
       </c>
-    </row>
-    <row r="35" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B35" s="3" t="s">
+      <c r="M35" s="31">
+        <v>81.421999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H35" s="38">
+      <c r="H36" s="29">
         <v>483.14800000000002</v>
       </c>
-      <c r="L35" s="38">
+      <c r="I36" s="29">
+        <v>627.10299999999995</v>
+      </c>
+      <c r="L36" s="29">
         <v>697.47400000000005</v>
       </c>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B36" s="1" t="s">
+      <c r="M36" s="29">
+        <v>743.57899999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H37" s="31">
         <v>196.07</v>
       </c>
-      <c r="L36" s="40">
+      <c r="I37" s="31">
+        <v>203.21299999999999</v>
+      </c>
+      <c r="L37" s="31">
         <v>220.90100000000001</v>
       </c>
-    </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B37" s="1" t="s">
+      <c r="M37" s="31">
+        <v>226.28</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H37" s="40">
-        <f>SUM(H32:H36)</f>
+      <c r="H38" s="31">
+        <f>SUM(H33:H37)</f>
         <v>1395.413</v>
       </c>
-      <c r="L37" s="40">
-        <f>SUM(L32:L36)</f>
+      <c r="I38" s="31">
+        <f>SUM(I33:I37)</f>
+        <v>1369.2529999999999</v>
+      </c>
+      <c r="L38" s="31">
+        <f>SUM(L33:L37)</f>
         <v>1267.434</v>
       </c>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B38" s="1" t="s">
+      <c r="M38" s="31">
+        <f>SUM(M33:M37)</f>
+        <v>1345.0759999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="H38" s="40">
+      <c r="H39" s="31">
         <v>1047.751</v>
       </c>
-      <c r="L38" s="40">
+      <c r="I39" s="31">
+        <v>1088.287</v>
+      </c>
+      <c r="L39" s="31">
         <v>1150.2470000000001</v>
       </c>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B39" s="1" t="s">
+      <c r="M39" s="31">
+        <v>1175.08</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="H39" s="40">
+      <c r="H40" s="31">
         <v>1068.9190000000001</v>
       </c>
-      <c r="L39" s="40">
+      <c r="I40" s="31">
+        <v>1030.7760000000001</v>
+      </c>
+      <c r="L40" s="31">
         <v>927.68499999999995</v>
       </c>
-    </row>
-    <row r="40" spans="2:12" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B40" s="3" t="s">
+      <c r="M40" s="31">
+        <v>927.09199999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H40" s="38">
+      <c r="H41" s="29">
         <v>113.249</v>
       </c>
-      <c r="L40" s="38">
+      <c r="I41" s="29">
+        <v>269.77999999999997</v>
+      </c>
+      <c r="L41" s="29">
         <v>152.52799999999999</v>
       </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B41" s="1" t="s">
+      <c r="M41" s="29">
+        <v>95.245999999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H41" s="40">
+      <c r="H42" s="31">
         <v>117.556</v>
       </c>
-      <c r="L41" s="40">
+      <c r="I42" s="31">
+        <v>132.51</v>
+      </c>
+      <c r="L42" s="31">
         <v>155.53800000000001</v>
       </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B42" s="1" t="s">
+      <c r="M42" s="31">
+        <v>177.62200000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="40">
-        <f>SUM(H38:H41)+H37</f>
+      <c r="H43" s="31">
+        <f>SUM(H39:H42)+H38</f>
         <v>3742.8879999999999</v>
       </c>
-      <c r="L42" s="40">
-        <f>SUM(L38:L41)+L37</f>
+      <c r="I43" s="31">
+        <f>SUM(I39:I42)+I38</f>
+        <v>3890.6059999999998</v>
+      </c>
+      <c r="L43" s="31">
+        <f>SUM(L39:L42)+L38</f>
         <v>3653.4319999999998</v>
       </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="H43" s="40"/>
-      <c r="L43" s="40"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B44" s="1" t="s">
+      <c r="M43" s="31">
+        <f>SUM(M39:M42)+M38</f>
+        <v>3720.116</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="40">
+      <c r="H45" s="31">
         <v>240.245</v>
       </c>
-      <c r="L44" s="40">
+      <c r="I45" s="31">
+        <v>315.48099999999999</v>
+      </c>
+      <c r="L45" s="31">
         <v>347.80500000000001</v>
       </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B45" s="1" t="s">
+      <c r="M45" s="31">
+        <v>326.529</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="40">
+      <c r="H46" s="31">
         <v>243.33799999999999</v>
       </c>
-      <c r="L45" s="40">
+      <c r="I46" s="31">
+        <v>240.07400000000001</v>
+      </c>
+      <c r="L46" s="31">
         <v>222.43</v>
       </c>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B46" s="1" t="s">
+      <c r="M46" s="31">
+        <v>224.37799999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H46" s="40">
+      <c r="H47" s="31">
         <v>462.78199999999998</v>
       </c>
-      <c r="L46" s="40">
+      <c r="I47" s="31">
+        <v>493.44600000000003</v>
+      </c>
+      <c r="L47" s="31">
         <v>396.65</v>
       </c>
-    </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B47" s="1" t="s">
+      <c r="M47" s="31">
+        <v>457.53699999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="H47" s="40">
-        <f>SUM(H44:H46)</f>
+      <c r="H48" s="31">
+        <f>SUM(H45:H47)</f>
         <v>946.36500000000001</v>
       </c>
-      <c r="L47" s="40">
-        <f>SUM(L44:L46)</f>
+      <c r="I48" s="31">
+        <f>SUM(I45:I47)</f>
+        <v>1049.0010000000002</v>
+      </c>
+      <c r="L48" s="31">
+        <f>SUM(L45:L47)</f>
         <v>966.88499999999999</v>
       </c>
-    </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B48" s="1" t="s">
+      <c r="M48" s="31">
+        <f>SUM(M45:M47)</f>
+        <v>1008.444</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H48" s="40">
+      <c r="H49" s="31">
         <v>1030.212</v>
       </c>
-      <c r="L48" s="40">
+      <c r="I49" s="31">
+        <v>986.02599999999995</v>
+      </c>
+      <c r="L49" s="31">
         <v>868.68600000000004</v>
       </c>
-    </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B49" s="1" t="s">
+      <c r="M49" s="31">
+        <v>861.03300000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="H49" s="40">
+      <c r="H50" s="31">
         <v>96.891000000000005</v>
       </c>
-      <c r="L49" s="40">
+      <c r="I50" s="31">
+        <v>108.848</v>
+      </c>
+      <c r="L50" s="31">
         <v>110.669</v>
       </c>
-    </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B50" s="1" t="s">
+      <c r="M50" s="31">
+        <v>112.248</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H50" s="40">
-        <f>H47+SUM(H48:H49)</f>
+      <c r="H51" s="31">
+        <f>H48+SUM(H49:H50)</f>
         <v>2073.4679999999998</v>
       </c>
-      <c r="L50" s="40">
-        <f>L47+SUM(L48:L49)</f>
+      <c r="I51" s="31">
+        <f>I48+SUM(I49:I50)</f>
+        <v>2143.875</v>
+      </c>
+      <c r="L51" s="31">
+        <f>L48+SUM(L49:L50)</f>
         <v>1946.24</v>
       </c>
-    </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="H51" s="40"/>
-    </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B52" s="1" t="s">
+      <c r="M51" s="31">
+        <f>M48+SUM(M49:M50)</f>
+        <v>1981.7249999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H52" s="31"/>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H52" s="40">
+      <c r="H53" s="31">
         <v>1669.42</v>
       </c>
-      <c r="L52" s="40">
+      <c r="I53" s="31">
+        <v>1746.731</v>
+      </c>
+      <c r="L53" s="31">
         <v>1707.192</v>
       </c>
-    </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B53" s="1" t="s">
+      <c r="M53" s="31">
+        <v>1738.3910000000001</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="H53" s="40">
-        <f>H52+H50</f>
+      <c r="H54" s="31">
+        <f>H53+H51</f>
         <v>3742.8879999999999</v>
       </c>
-      <c r="L53" s="40">
-        <f>L52+L50</f>
+      <c r="I54" s="31">
+        <f>I53+I51</f>
+        <v>3890.6059999999998</v>
+      </c>
+      <c r="L54" s="31">
+        <f>L53+L51</f>
         <v>3653.4319999999998</v>
       </c>
-    </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="L54" s="40"/>
-    </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B55" s="1" t="s">
+      <c r="M54" s="31">
+        <f>M53+M51</f>
+        <v>3720.116</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L55" s="31"/>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="H55" s="40">
-        <f>H42-H50</f>
+      <c r="H56" s="31">
+        <f>H43-H51</f>
         <v>1669.42</v>
       </c>
-      <c r="L55" s="40">
-        <f>L42-L50</f>
+      <c r="I56" s="31">
+        <f t="shared" ref="I56" si="9">I43-I51</f>
+        <v>1746.7309999999998</v>
+      </c>
+      <c r="L56" s="31">
+        <f>L43-L51</f>
         <v>1707.1919999999998</v>
       </c>
-    </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B56" s="1" t="s">
+      <c r="M56" s="31">
+        <f t="shared" ref="M56" si="10">M43-M51</f>
+        <v>1738.3910000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="H56" s="1">
-        <f>H55/H19</f>
+      <c r="H57" s="1">
+        <f>H56/H20</f>
         <v>16.980242198171087</v>
       </c>
-      <c r="L56" s="1">
-        <f>L55/L19</f>
+      <c r="I57" s="1">
+        <f t="shared" ref="I57" si="11">I56/I20</f>
+        <v>17.787050192124124</v>
+      </c>
+      <c r="L57" s="1">
+        <f>L56/L20</f>
         <v>18.348752828179222</v>
       </c>
-    </row>
-    <row r="58" spans="2:12" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B58" s="37" t="s">
+      <c r="M57" s="1">
+        <f t="shared" ref="M57" si="12">M56/M20</f>
+        <v>18.859851828321517</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="H58" s="39">
-        <f>H32+H33+H40</f>
+      <c r="H59" s="30">
+        <f>H33+H34+H41</f>
         <v>735.04200000000003</v>
       </c>
-      <c r="L58" s="39">
-        <f>L32+L33+L40</f>
+      <c r="I59" s="30">
+        <f t="shared" ref="I59" si="13">I33+I34+I41</f>
+        <v>694.50900000000001</v>
+      </c>
+      <c r="L59" s="30">
+        <f>L33+L34+L41</f>
         <v>404.21299999999997</v>
       </c>
-    </row>
-    <row r="59" spans="2:12" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B59" s="37" t="s">
+      <c r="M59" s="30">
+        <f t="shared" ref="M59" si="14">M33+M34+M41</f>
+        <v>389.041</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" s="28" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B60" s="1" t="s">
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B61" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H60" s="40">
-        <f>H58-H59</f>
+      <c r="H61" s="31">
+        <f>H59-H60</f>
         <v>735.04200000000003</v>
       </c>
-      <c r="L60" s="40">
-        <f>L58-L59</f>
+      <c r="I61" s="31">
+        <f t="shared" ref="I61" si="15">I59-I60</f>
+        <v>694.50900000000001</v>
+      </c>
+      <c r="L61" s="31">
+        <f>L59-L60</f>
         <v>404.21299999999997</v>
       </c>
-    </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B62" s="1" t="s">
+      <c r="M61" s="31">
+        <f t="shared" ref="M61" si="16">M59-M60</f>
+        <v>389.041</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B63" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="L62" s="46">
-        <f>L35/H35-1</f>
+      <c r="L63" s="37">
+        <f>L36/H36-1</f>
         <v>0.44360320233137673</v>
       </c>
-    </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B63" s="1" t="s">
+      <c r="M63" s="37">
+        <f>M36/I36-1</f>
+        <v>0.18573663337601642</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B64" s="1" t="s">
+      <c r="I64" s="37">
+        <f>I36/H36-1</f>
+        <v>0.29795218028430193</v>
+      </c>
+      <c r="M64" s="37">
+        <f>M36/L36-1</f>
+        <v>6.610282247080157E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B66" s="1" t="s">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H67" s="1">
         <v>37.18</v>
       </c>
-      <c r="L66" s="1">
+      <c r="I67" s="1">
+        <v>31.93</v>
+      </c>
+      <c r="L67" s="1">
         <v>20.53</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B67" s="1" t="s">
+      <c r="M67" s="1">
+        <v>23.86</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H67" s="40">
-        <f>H66*H19</f>
+      <c r="H68" s="31">
+        <f>H67*H20</f>
         <v>3655.3680963800002</v>
       </c>
-      <c r="L67" s="40">
-        <f>L66*L19</f>
+      <c r="I68" s="31">
+        <f t="shared" ref="I68" si="17">I67*I20</f>
+        <v>3135.6026000699999</v>
+      </c>
+      <c r="L68" s="31">
+        <f>L67*L20</f>
         <v>1910.1380942999999</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B68" s="1" t="s">
+      <c r="M68" s="31">
+        <f t="shared" ref="M68" si="18">M67*M20</f>
+        <v>2199.2754575999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H68" s="40">
-        <f>H67-H60</f>
+      <c r="H69" s="31">
+        <f>H68-H61</f>
         <v>2920.3260963800003</v>
       </c>
-      <c r="L68" s="40">
-        <f>L67-L60</f>
+      <c r="I69" s="31">
+        <f t="shared" ref="I69" si="19">I68-I61</f>
+        <v>2441.0936000699999</v>
+      </c>
+      <c r="L69" s="31">
+        <f>L68-L61</f>
         <v>1505.9250943</v>
       </c>
-    </row>
-    <row r="70" spans="1:12" s="53" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="54">
-        <f>AVERAGE(C70:L70)</f>
-        <v>1.6542403839438049</v>
-      </c>
-      <c r="B70" s="53" t="s">
+      <c r="M69" s="31">
+        <f t="shared" ref="M69" si="20">M68-M61</f>
+        <v>1810.2344575999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="41">
+        <f>AVERAGE(C71:L71)</f>
+        <v>1.701202325991255</v>
+      </c>
+      <c r="B71" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="H70" s="53">
-        <f>H66/H56</f>
+      <c r="H71" s="40">
+        <f>H67/H57</f>
         <v>2.1896036326269006</v>
       </c>
-      <c r="L70" s="53">
-        <f>L66/L56</f>
+      <c r="I71" s="40">
+        <f>I67/I57</f>
+        <v>1.7951262100861554</v>
+      </c>
+      <c r="L71" s="40">
+        <f>L67/L57</f>
         <v>1.118877135260709</v>
       </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B71" s="1" t="s">
+      <c r="M71" s="40">
+        <f>M67/M57</f>
+        <v>1.2651212860628016</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B72" s="1" t="s">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B73" s="1" t="s">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="B74" s="1" t="s">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B75" s="1" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2256,12 +2632,13 @@
   <phoneticPr fontId="9" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="L1" r:id="rId1" xr:uid="{A150210D-96D1-0642-91C1-FA5095E7FDDD}"/>
+    <hyperlink ref="M1" r:id="rId2" xr:uid="{9A4CB837-4115-4EBE-B3F4-3C5DD1EE34BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="L9" formulaRange="1"/>
+    <ignoredError sqref="L9:M9" formulaRange="1"/>
   </ignoredErrors>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>